<commit_message>
Work on Code Gen, just add a security when nobody set analogic function to not launch conversion
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32F030R8/STM32F030R8_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32F030R8/STM32F030R8_HwCfg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\fAnalogSignal\Doc\ConfigPrj\ExcelCfg\STM32F030R8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A9B546-D67F-4CB6-956F-9F5F2AF5AC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38046D9E-E6C5-4BEB-ADDA-B17BC4289B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="232">
   <si>
     <t>Colonne1</t>
   </si>
@@ -810,7 +810,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1060,19 +1060,21 @@
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}" name="FMKCDA_CalibrationOthers" displayName="FMKCDA_CalibrationOthers" ref="I3:J4" totalsRowShown="0">
-  <autoFilter ref="I3:J4" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}" name="FMKCDA_CalibrationOthers" displayName="FMKCDA_CalibrationOthers" ref="I3:L4" totalsRowShown="0">
+  <autoFilter ref="I3:L4" xr:uid="{A4F27ADC-56A6-479B-93EF-D6AA72368D72}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{74AD6856-B046-40F9-89E8-C5AC0EB4C661}" name="calibration temperature "/>
     <tableColumn id="2" xr3:uid="{D58B2B24-74EC-4445-9DDA-83A119877B67}" name="address in hexacecimal"/>
+    <tableColumn id="3" xr3:uid="{0793AAF2-321B-4695-AEBB-122FAB9D49F7}" name="Adc Vref"/>
+    <tableColumn id="4" xr3:uid="{F1198D75-5BAD-4CA5-814F-DDA2BB66E5F2}" name="Channel Vref"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}" name="FMKCDA_VoltageRef" displayName="FMKCDA_VoltageRef" ref="Q3:T4" totalsRowShown="0">
-  <autoFilter ref="Q3:T4" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}" name="FMKCDA_VoltageRef" displayName="FMKCDA_VoltageRef" ref="S3:V4" totalsRowShown="0">
+  <autoFilter ref="S3:V4" xr:uid="{99B4503A-67B2-48AD-BE25-2B3425F892A9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0BCC2BC4-7FF0-4C14-809D-9D95A3225151}" name="Vref Calib"/>
     <tableColumn id="2" xr3:uid="{0E78A6D4-DF9E-4966-A80E-64FE5BD9F1E2}" name="address  hexacecimal" dataDxfId="0"/>
@@ -1478,7 +1480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
   <dimension ref="A15:AA43"/>
   <sheetViews>
-    <sheetView topLeftCell="J9" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="H9" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="S40" sqref="S38:AA40"/>
     </sheetView>
   </sheetViews>
@@ -3127,24 +3129,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0962FBCC-E1F3-44E3-92A8-D1FF17927B08}">
-  <dimension ref="I2:T4"/>
+  <dimension ref="I2:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="9" max="9" width="43.88671875" customWidth="1"/>
     <col min="10" max="10" width="21.6640625" customWidth="1"/>
-    <col min="11" max="12" width="11.5546875" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" customWidth="1"/>
+    <col min="12" max="12" width="24.109375" customWidth="1"/>
     <col min="17" max="17" width="45" customWidth="1"/>
     <col min="18" max="18" width="28.88671875" customWidth="1"/>
     <col min="19" max="19" width="21.88671875" customWidth="1"/>
     <col min="20" max="20" width="19.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="9:20" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="9:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I2" s="3" t="s">
         <v>225</v>
       </c>
@@ -3152,43 +3155,55 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="9:22" x14ac:dyDescent="0.3">
       <c r="I3" t="s">
         <v>221</v>
       </c>
       <c r="J3" t="s">
         <v>228</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="K3" t="s">
+        <v>226</v>
+      </c>
+      <c r="L3" t="s">
+        <v>227</v>
+      </c>
+      <c r="S3" t="s">
         <v>224</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>229</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>226</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="9:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="9:22" x14ac:dyDescent="0.3">
       <c r="I4" t="s">
         <v>220</v>
       </c>
       <c r="J4" t="s">
         <v>231</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
+        <v>178</v>
+      </c>
+      <c r="S4" t="s">
         <v>223</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
         <v>17</v>
       </c>
-      <c r="T4" t="s">
+      <c r="V4" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3201,18 +3216,24 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7AB0981D-B484-49AA-81E2-46EA728857EF}">
           <x14:formula1>
             <xm:f>FMK_IO!$AN$6:$AN$23</xm:f>
           </x14:formula1>
-          <xm:sqref>T4</xm:sqref>
+          <xm:sqref>V4 L4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6F78BF8D-EC95-4E4B-B9DE-1CEC06FF7E2D}">
           <x14:formula1>
-            <xm:f>General_Info!P19</xm:f>
+            <xm:f>General_Info!R19</xm:f>
           </x14:formula1>
-          <xm:sqref>S4</xm:sqref>
+          <xm:sqref>U4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9E258101-4BE3-4FFA-9159-E0120D35AA71}">
+          <x14:formula1>
+            <xm:f>General_Info!$P$19</xm:f>
+          </x14:formula1>
+          <xm:sqref>K4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Finished module CDA, Update GenCode, Make.bat
</commit_message>
<xml_diff>
--- a/Doc/ConfigPrj/ExcelCfg/STM32F030R8/STM32F030R8_HwCfg.xlsx
+++ b/Doc/ConfigPrj/ExcelCfg/STM32F030R8/STM32F030R8_HwCfg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Software\STM32\fAnalogSignal\Doc\ConfigPrj\ExcelCfg\STM32F030R8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38046D9E-E6C5-4BEB-ADDA-B17BC4289B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF33399-7B71-49B9-BE54-C7D0B94C16CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2AF09063-600F-437A-B138-F66136E922A5}"/>
   </bookViews>
   <sheets>
     <sheet name="General_Info" sheetId="1" r:id="rId1"/>
@@ -491,12 +491,6 @@
     <t>Clock for Power Control register access.</t>
   </si>
   <si>
-    <t>STM32 Family</t>
-  </si>
-  <si>
-    <t>STM32 Process</t>
-  </si>
-  <si>
     <t>_NVIC_Piority_Choice</t>
   </si>
   <si>
@@ -735,6 +729,12 @@
   </si>
   <si>
     <t>0x1FFFF7BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM32 Processor </t>
+  </si>
+  <si>
+    <t>stm32f030x8</t>
   </si>
 </sst>
 </file>
@@ -1141,21 +1141,20 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{69B16F87-38FA-4931-845E-91EC8B0FFB29}" name="Tableau5" displayName="Tableau5" ref="A15:B16" totalsRowShown="0">
-  <autoFilter ref="A15:B16" xr:uid="{69B16F87-38FA-4931-845E-91EC8B0FFB29}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FD4FECA3-1A39-43C0-8443-3217FDF815FF}" name="STM32 Family"/>
-    <tableColumn id="2" xr3:uid="{DDA90C22-9D42-40D5-A8DF-C1879E8D680C}" name="STM32 Process"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}" name="Tableau16" displayName="Tableau16" ref="AA17:AA20" totalsRowShown="0">
+  <autoFilter ref="AA17:AA20" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{84137467-8FB1-43EA-9F20-573D7FE9FADD}" name="_NVIC_Piority_Choice"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}" name="Tableau16" displayName="Tableau16" ref="AA17:AA20" totalsRowShown="0">
-  <autoFilter ref="AA17:AA20" xr:uid="{13E9277E-229F-41F0-9B99-7D1A0B71D1B3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{69B16F87-38FA-4931-845E-91EC8B0FFB29}" name="CPU_Config" displayName="CPU_Config" ref="B18:B19" totalsRowShown="0">
+  <autoFilter ref="B18:B19" xr:uid="{69B16F87-38FA-4931-845E-91EC8B0FFB29}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{84137467-8FB1-43EA-9F20-573D7FE9FADD}" name="_NVIC_Piority_Choice"/>
+    <tableColumn id="1" xr3:uid="{FD4FECA3-1A39-43C0-8443-3217FDF815FF}" name="STM32 Processor "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1478,16 +1477,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871E2D6D-43F7-44B1-8255-ECFDDA33AA9C}">
-  <dimension ref="A15:AA43"/>
+  <dimension ref="B17:AA43"/>
   <sheetViews>
-    <sheetView topLeftCell="H9" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S40" sqref="S38:AA40"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" customWidth="1"/>
     <col min="3" max="3" width="37.33203125" customWidth="1"/>
     <col min="4" max="4" width="81" customWidth="1"/>
     <col min="5" max="5" width="85.109375" customWidth="1"/>
@@ -1507,20 +1506,15 @@
     <col min="27" max="27" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="17" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="AA17" t="s">
         <v>150</v>
       </c>
-      <c r="B15" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="4:27" x14ac:dyDescent="0.3">
-      <c r="AA17" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="4:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>230</v>
+      </c>
       <c r="D18" t="s">
         <v>25</v>
       </c>
@@ -1564,10 +1558,13 @@
         <v>19</v>
       </c>
       <c r="AA18" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="19" spans="4:27" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>231</v>
+      </c>
       <c r="D19" t="s">
         <v>104</v>
       </c>
@@ -1614,7 +1611,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>105</v>
       </c>
@@ -1640,10 +1637,10 @@
         <v>16</v>
       </c>
       <c r="AA20" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="21" spans="4:27" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>106</v>
       </c>
@@ -1669,7 +1666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>107</v>
       </c>
@@ -1695,7 +1692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>108</v>
       </c>
@@ -1721,7 +1718,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>109</v>
       </c>
@@ -1741,7 +1738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>110</v>
       </c>
@@ -1755,7 +1752,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>111</v>
       </c>
@@ -1769,7 +1766,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>112</v>
       </c>
@@ -1783,7 +1780,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>113</v>
       </c>
@@ -1797,7 +1794,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>114</v>
       </c>
@@ -1811,7 +1808,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>115</v>
       </c>
@@ -1825,7 +1822,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>116</v>
       </c>
@@ -1839,7 +1836,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="4:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:27" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
         <v>117</v>
       </c>
@@ -2047,7 +2044,7 @@
   <sheetData>
     <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.3">
@@ -2111,7 +2108,7 @@
         <v>90</v>
       </c>
       <c r="AJ5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AN5" t="s">
         <v>56</v>
@@ -2170,7 +2167,7 @@
         <v>23</v>
       </c>
       <c r="U6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="W6" t="s">
         <v>14</v>
@@ -2188,7 +2185,7 @@
         <v>51</v>
       </c>
       <c r="AB6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AD6" t="s">
         <v>13</v>
@@ -2197,16 +2194,16 @@
         <v>42</v>
       </c>
       <c r="AF6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="AJ6" t="s">
         <v>29</v>
       </c>
       <c r="AL6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AN6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.3">
@@ -2229,10 +2226,10 @@
         <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K7" t="s">
         <v>12</v>
@@ -2280,7 +2277,7 @@
         <v>52</v>
       </c>
       <c r="AB7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AD7" t="s">
         <v>13</v>
@@ -2289,7 +2286,7 @@
         <v>43</v>
       </c>
       <c r="AF7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="AJ7" t="s">
         <v>30</v>
@@ -2298,7 +2295,7 @@
         <v>51</v>
       </c>
       <c r="AN7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.3">
@@ -2321,10 +2318,10 @@
         <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K8" t="s">
         <v>13</v>
@@ -2342,7 +2339,7 @@
         <v>51</v>
       </c>
       <c r="P8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="W8" t="s">
         <v>14</v>
@@ -2357,10 +2354,10 @@
         <v>5</v>
       </c>
       <c r="AA8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AB8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AD8" t="s">
         <v>14</v>
@@ -2369,7 +2366,7 @@
         <v>33</v>
       </c>
       <c r="AF8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="AJ8" t="s">
         <v>31</v>
@@ -2378,7 +2375,7 @@
         <v>52</v>
       </c>
       <c r="AN8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.3">
@@ -2389,7 +2386,7 @@
         <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -2401,10 +2398,10 @@
         <v>17</v>
       </c>
       <c r="H9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K9" t="s">
         <v>13</v>
@@ -2422,7 +2419,7 @@
         <v>52</v>
       </c>
       <c r="P9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="W9" t="s">
         <v>14</v>
@@ -2440,7 +2437,7 @@
         <v>57</v>
       </c>
       <c r="AB9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AD9" t="s">
         <v>14</v>
@@ -2449,16 +2446,16 @@
         <v>34</v>
       </c>
       <c r="AF9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="AJ9" t="s">
         <v>32</v>
       </c>
       <c r="AL9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AN9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.3">
@@ -2469,7 +2466,7 @@
         <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -2481,10 +2478,10 @@
         <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="W10" t="s">
         <v>12</v>
@@ -2511,7 +2508,7 @@
         <v>43</v>
       </c>
       <c r="AF10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="AJ10" t="s">
         <v>33</v>
@@ -2520,7 +2517,7 @@
         <v>57</v>
       </c>
       <c r="AN10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.3">
@@ -2531,7 +2528,7 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -2543,7 +2540,7 @@
         <v>17</v>
       </c>
       <c r="H11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I11" t="s">
         <v>96</v>
@@ -2573,13 +2570,13 @@
         <v>33</v>
       </c>
       <c r="AF11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AJ11" t="s">
         <v>34</v>
       </c>
       <c r="AN11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.3">
@@ -2590,7 +2587,7 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -2602,13 +2599,13 @@
         <v>17</v>
       </c>
       <c r="H12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I12" t="s">
         <v>97</v>
       </c>
       <c r="T12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="W12" t="s">
         <v>12</v>
@@ -2623,7 +2620,7 @@
         <v>4</v>
       </c>
       <c r="AA12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AB12" t="s">
         <v>100</v>
@@ -2635,13 +2632,13 @@
         <v>34</v>
       </c>
       <c r="AF12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="AJ12" t="s">
         <v>35</v>
       </c>
       <c r="AN12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.3">
@@ -2652,7 +2649,7 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -2664,10 +2661,10 @@
         <v>17</v>
       </c>
       <c r="H13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I13" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="W13" t="s">
         <v>12</v>
@@ -2694,13 +2691,13 @@
         <v>35</v>
       </c>
       <c r="AF13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AJ13" t="s">
         <v>36</v>
       </c>
       <c r="AN13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.3">
@@ -2711,7 +2708,7 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
@@ -2723,10 +2720,10 @@
         <v>17</v>
       </c>
       <c r="H14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="AD14" t="s">
         <v>16</v>
@@ -2735,13 +2732,13 @@
         <v>36</v>
       </c>
       <c r="AF14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="AJ14" t="s">
         <v>37</v>
       </c>
       <c r="AN14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.3">
@@ -2752,7 +2749,7 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -2764,7 +2761,7 @@
         <v>17</v>
       </c>
       <c r="H15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I15" t="s">
         <v>92</v>
@@ -2773,7 +2770,7 @@
         <v>38</v>
       </c>
       <c r="AN15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.3">
@@ -2784,7 +2781,7 @@
         <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -2796,7 +2793,7 @@
         <v>17</v>
       </c>
       <c r="H16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I16" t="s">
         <v>93</v>
@@ -2805,7 +2802,7 @@
         <v>39</v>
       </c>
       <c r="AN16" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.3">
@@ -2816,13 +2813,13 @@
         <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AJ17" t="s">
         <v>40</v>
       </c>
       <c r="AN17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.3">
@@ -2830,7 +2827,7 @@
         <v>42</v>
       </c>
       <c r="AN18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.3">
@@ -2838,7 +2835,7 @@
         <v>43</v>
       </c>
       <c r="AN19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.3">
@@ -2846,7 +2843,7 @@
         <v>44</v>
       </c>
       <c r="AN20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.3">
@@ -2854,22 +2851,22 @@
         <v>45</v>
       </c>
       <c r="AN21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AN22" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AN23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.3">
@@ -2880,7 +2877,7 @@
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.3">
@@ -2894,13 +2891,13 @@
         <v>95</v>
       </c>
       <c r="E26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M26" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.3">
@@ -2920,7 +2917,7 @@
         <v>28</v>
       </c>
       <c r="G27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I27" t="s">
         <v>27</v>
@@ -2929,7 +2926,7 @@
         <v>28</v>
       </c>
       <c r="K27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M27" t="s">
         <v>27</v>
@@ -2938,7 +2935,7 @@
         <v>28</v>
       </c>
       <c r="O27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.3">
@@ -2958,7 +2955,7 @@
         <v>35</v>
       </c>
       <c r="G28" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I28" t="s">
         <v>14</v>
@@ -2967,7 +2964,7 @@
         <v>39</v>
       </c>
       <c r="K28" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="M28" t="s">
         <v>12</v>
@@ -2976,7 +2973,7 @@
         <v>29</v>
       </c>
       <c r="O28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.3">
@@ -2987,7 +2984,7 @@
         <v>36</v>
       </c>
       <c r="G29" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I29" t="s">
         <v>14</v>
@@ -2996,7 +2993,7 @@
         <v>40</v>
       </c>
       <c r="K29" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M29" t="s">
         <v>12</v>
@@ -3005,7 +3002,7 @@
         <v>44</v>
       </c>
       <c r="O29" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.3">
@@ -3016,7 +3013,7 @@
         <v>42</v>
       </c>
       <c r="K30" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M30" t="s">
         <v>12</v>
@@ -3025,7 +3022,7 @@
         <v>45</v>
       </c>
       <c r="O30" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -3131,7 +3128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0962FBCC-E1F3-44E3-92A8-D1FF17927B08}">
   <dimension ref="I2:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -3149,62 +3146,62 @@
   <sheetData>
     <row r="2" spans="9:22" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I2" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="9:22" x14ac:dyDescent="0.3">
       <c r="I3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="L3" t="s">
+        <v>225</v>
+      </c>
+      <c r="S3" t="s">
+        <v>222</v>
+      </c>
+      <c r="T3" t="s">
         <v>227</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>224</v>
       </c>
-      <c r="T3" t="s">
-        <v>229</v>
-      </c>
-      <c r="U3" t="s">
-        <v>226</v>
-      </c>
       <c r="V3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="9:22" x14ac:dyDescent="0.3">
       <c r="I4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K4" t="s">
         <v>17</v>
       </c>
       <c r="L4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="S4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U4" t="s">
         <v>17</v>
       </c>
       <c r="V4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -3223,18 +3220,18 @@
           </x14:formula1>
           <xm:sqref>V4 L4</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9E258101-4BE3-4FFA-9159-E0120D35AA71}">
+          <x14:formula1>
+            <xm:f>General_Info!$P$19</xm:f>
+          </x14:formula1>
+          <xm:sqref>K4</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6F78BF8D-EC95-4E4B-B9DE-1CEC06FF7E2D}">
           <x14:formula1>
             <xm:f>General_Info!R19</xm:f>
           </x14:formula1>
           <xm:sqref>U4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9E258101-4BE3-4FFA-9159-E0120D35AA71}">
-          <x14:formula1>
-            <xm:f>General_Info!$P$19</xm:f>
-          </x14:formula1>
-          <xm:sqref>K4</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>

</xml_diff>